<commit_message>
added test for limit_surplus carry through
</commit_message>
<xml_diff>
--- a/ftest/data/fm48/Max.Ded.Calculation.Example.xlsx
+++ b/ftest/data/fm48/Max.Ded.Calculation.Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\ktest\ftest\data\fm48\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\ktest\ftest\data\fm48\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A65C2A6-706C-46B4-819A-47D588E19FB7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69556D7D-1E99-436C-880D-E09B751F11F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1920" windowWidth="23040" windowHeight="8964" activeTab="1" xr2:uid="{75D5E7CF-EFFD-4508-9A5B-71E86028FB54}"/>
+    <workbookView xWindow="-6852" yWindow="-336" windowWidth="17280" windowHeight="8916" activeTab="1" xr2:uid="{75D5E7CF-EFFD-4508-9A5B-71E86028FB54}"/>
   </bookViews>
   <sheets>
     <sheet name="MaxDed_old" sheetId="2" r:id="rId1"/>
@@ -22,12 +22,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
   <si>
     <t>Location</t>
   </si>
@@ -126,6 +131,30 @@
   </si>
   <si>
     <t>e.g. in example below gross loss is 600,000 - even though MaxDed has decreased the level of the deductibles -  the full location limits still apply</t>
+  </si>
+  <si>
+    <t>x.loss</t>
+  </si>
+  <si>
+    <t>deductible</t>
+  </si>
+  <si>
+    <t>loss</t>
+  </si>
+  <si>
+    <t>accumulated_limit</t>
+  </si>
+  <si>
+    <t>x.limit_surplus</t>
+  </si>
+  <si>
+    <t>x.effective_deductible</t>
+  </si>
+  <si>
+    <t>adjusted limit_surplus</t>
+  </si>
+  <si>
+    <t>loss_adj</t>
   </si>
 </sst>
 </file>
@@ -192,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -215,6 +244,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,18 +919,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF30DA28-3D8C-42F1-9C20-4F304D5C63B5}">
-  <dimension ref="B2:F36"/>
+  <dimension ref="B2:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="54.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="18" x14ac:dyDescent="0.35">
@@ -1020,7 +1052,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>4</v>
       </c>
@@ -1031,19 +1063,19 @@
       <c r="E17" s="4"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1052,7 +1084,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1060,7 +1092,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>8</v>
       </c>
@@ -1081,7 +1113,7 @@
         <v>1250000</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>10</v>
       </c>
@@ -1102,7 +1134,7 @@
         <v>1247000</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>11</v>
       </c>
@@ -1123,7 +1155,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>12</v>
       </c>
@@ -1144,7 +1176,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="7" t="s">
         <v>24</v>
       </c>
@@ -1165,13 +1197,13 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>13</v>
       </c>
@@ -1182,14 +1214,16 @@
         <f>F25</f>
         <v>600000</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>17</v>
       </c>
@@ -1201,7 +1235,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" s="7" t="s">
         <v>25</v>
       </c>
@@ -1213,7 +1247,7 @@
         <v>602000</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32" s="7" t="s">
         <v>26</v>
       </c>
@@ -1269,6 +1303,80 @@
         <f>F34</f>
         <v>600000</v>
       </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="10">
+        <f>F28</f>
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="10">
+        <f>F23-F26</f>
+        <v>647000</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="10">
+        <f>F24</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="10">
+        <f>C16</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="10">
+        <f>C38+C40-C41</f>
+        <v>602000</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="10">
+        <f>IF(C39&gt;0,C38)</f>
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="10">
+        <f>C42-C38</f>
+        <v>2000</v>
+      </c>
+      <c r="F44" s="10"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" s="10">
+        <f>C39+C44</f>
+        <v>649000</v>
+      </c>
+      <c r="F45" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>